<commit_message>
Updated models and added steps to set-up guide
</commit_message>
<xml_diff>
--- a/modelos/modelo_normal.xlsx
+++ b/modelos/modelo_normal.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510329B6-FF87-44C9-87FB-91B4E999ACB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5E27E8-698F-4859-A688-78A392BFC0C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,21 +37,6 @@
     <t>Número:</t>
   </si>
   <si>
-    <t>ALSEFIN &amp; ASOCIADOS</t>
-  </si>
-  <si>
-    <t>Alvaro Luche Sánchez</t>
-  </si>
-  <si>
-    <t>Calle Menorca 10, Semi Sotano Int. Izda.</t>
-  </si>
-  <si>
-    <t>28009 Madrid</t>
-  </si>
-  <si>
-    <t>NIF: 50.844.986-J</t>
-  </si>
-  <si>
     <t>Comentarios:</t>
   </si>
   <si>
@@ -82,116 +70,6 @@
     <t>Fecha:</t>
   </si>
   <si>
-    <r>
-      <t>Le informamos que el Responsable del Tratamiento es</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ÁLVARO LUCHE SÁNCHEZ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">con domicilio a efecto de notificaciones en Madrid, CP 28009, C/ Menorca, nº 10, Semisótano Interior Izquierda, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>con la finalidad de gestionar la relación profesional, contable y fiscal</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. ÁLVARO LUCHE SÁNCHEZ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> se compromete a no ceder estos datos sin su previo consentimiento salvo aquellas cesiones que sean necesarios y se encuentren amparadas por las excepciones legalmente previstas. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ÁLVARO LUCHE SÁNCHEZ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> implantará las medidas de seguridad técnicas y organizativas necesarias para garantizar la seguridad de los datos de carácter personal de acuerdo con lo preceptuado en el RGPD, evitando de esta forma la pérdida, alteración y acceso no autorizado a los mismos. Le informamos también que puede ejercer los derechos de acceso, rectificación, oposición, supresión, limitación del tratamiento y portabilidad dirigiéndose por escrito a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ÁLVARO LUCHE SÁNCHEZ, en el domicilio indicado anteriormente. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Asimismo, en virtud de lo establecido en la Ley 34/2002, de 11 de julio, de Servicios de la Sociedad de la Información y de Comercio Electrónico le informamos que si usted ha autorizado el envío de novedades y noticias que puedan resultar de su interés utilizaremos las direcciones de correo electrónico facilitadas por usted para este fin.  No obstante si no desea recibir más información rogamos que nos envíe un correo electrónico .</t>
-    </r>
-  </si>
-  <si>
     <t>Firma y sello</t>
   </si>
   <si>
@@ -211,6 +89,24 @@
   </si>
   <si>
     <t>Forma de pago</t>
+  </si>
+  <si>
+    <t>COMPANY NAME</t>
+  </si>
+  <si>
+    <t>Person in charge</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>CP and City</t>
+  </si>
+  <si>
+    <t>NIF</t>
+  </si>
+  <si>
+    <t>Se republicae per mi Murmurabant dis Perpetuitas ex ARDUAS NEQUE HONOREM, nam mirabilia e fortes ea transtulissent ab Habeat, AB 58009, Y/ Rhoncus, pº 70, Contemptor Diabolum Occasione, eum id feliciora se concernit si subiecta coknbitandi, miseriae m tutela. HAERES MAGNA AVOCARE ac aversionem p ex earum culpa ipsam hic me indago deliberationes minus fundatam condigne cum esse supponebat v ex doloremque erubescam eum qui murmurabant bellicosum regulator. DEORUM SAEPE ARMORUM amplissima est encomia se scandalum commenti o irrevocabilem apostrophe quos combinatur te opprimere eu hic magni ab regnandi urgebant eu honorem nec in successione ab mi QUAM, delectus me enim magni at ferrens, fridericus d perare ab occidentem y dui leones. Ea adversitas tenetur hac earum exemplo est secundam ea proper, oportunitatis, sanguinis, proponent, effeminati est intestabunt e curiositatem oboedientiam eos lapidem p AENEAN RERUM CORPORE, ab in similique aliuando praetensionis. Zelabant, ac saluis ad te intendebant ea ut Rem 44/8002, ac 01 ea dicit, ab Passionis ea ut Condigne ad si Competentes v ad Nostramm Dignissimos at combinatur eos id nobis ea compellere si ipsum eu occumbere e fortiaue eos renovo tetnpore ac ac habetis expirationis vel malevolorum me amorem conditiones debilitatem rem porta quos quia tot.  Ad imperium mi eu eorum impetus sem aemulatione securus eos quo natus ex semper inventiones .</t>
   </si>
 </sst>
 </file>
@@ -220,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,14 +166,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.5"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="8.5"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -638,7 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -692,7 +580,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -705,13 +593,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -731,43 +649,13 @@
       <alignment horizontal="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -797,48 +685,50 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>377281</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>257013</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>178230</xdr:rowOff>
+      <xdr:rowOff>72494</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9274B9F0-2ADB-464D-A70D-AB04746DA607}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD20B10-3B0E-4F79-BA06-0AF03F82BB66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="5354" t="10700" r="5263" b="5589"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="2251801" y="0"/>
-          <a:ext cx="1731392" cy="1130730"/>
+          <a:off x="2689860" y="137160"/>
+          <a:ext cx="906780" cy="887834"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -846,71 +736,52 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>99850</xdr:colOff>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>10510</xdr:rowOff>
+      <xdr:rowOff>10880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>541284</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>141907</xdr:rowOff>
+      <xdr:rowOff>70291</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="0 Imagen" descr="Sello.jpg">
+        <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D33E50A7-CFB6-4EAC-9A60-39B738BA4C1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE0B7758-3088-485B-B528-5097559BE558}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="2003" t="2432"/>
-        <a:stretch/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="99850" y="8276896"/>
-          <a:ext cx="1697420" cy="1192942"/>
+          <a:off x="30480" y="8324300"/>
+          <a:ext cx="1920240" cy="1126211"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1186,8 +1057,8 @@
   </sheetPr>
   <dimension ref="A1:K294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48:K49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,26 +1068,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
       <c r="K1" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
       <c r="K2" s="8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K3" s="8" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1226,23 +1097,23 @@
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="K4" s="8" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="K5" s="8" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -1251,7 +1122,7 @@
       <c r="F7" s="26"/>
       <c r="G7" s="27"/>
       <c r="H7" s="14" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -1259,7 +1130,7 @@
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -1274,7 +1145,7 @@
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -1289,7 +1160,7 @@
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
@@ -1305,26 +1176,26 @@
     <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
+        <v>3</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="52"/>
-      <c r="J12" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="52"/>
+        <v>5</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="62"/>
+      <c r="J12" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
@@ -1821,64 +1692,64 @@
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="46">
+      <c r="D44" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="56">
         <f>SUM(J13:K42)</f>
         <v>0</v>
       </c>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
     </row>
     <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
       <c r="H46" s="22" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I46" s="40" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J46" s="40"/>
       <c r="K46" s="22" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
       <c r="H47" s="20">
         <v>0.21</v>
       </c>
@@ -1896,60 +1767,60 @@
       <c r="A48" s="6"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="60"/>
-      <c r="I48" s="60"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="61"/>
+      <c r="D48" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="46"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="51"/>
     </row>
     <row r="49" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="63"/>
-      <c r="K49" s="64"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="54"/>
     </row>
     <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="54">
+      <c r="D50" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="64">
         <f>I47+K47</f>
         <v>0</v>
       </c>
-      <c r="J50" s="54"/>
-      <c r="K50" s="54"/>
+      <c r="J50" s="64"/>
+      <c r="K50" s="64"/>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="17"/>
       <c r="C51" s="18"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="54"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="63"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="64"/>
     </row>
     <row r="52" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
@@ -1965,110 +1836,110 @@
       <c r="K52" s="15"/>
     </row>
     <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="45"/>
-      <c r="J53" s="45"/>
-      <c r="K53" s="45"/>
+      <c r="A53" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="55"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
+      <c r="H53" s="55"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="55"/>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="45"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="45"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="45"/>
+      <c r="A54" s="55"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
     </row>
     <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="45"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="45"/>
+      <c r="A55" s="55"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
     </row>
     <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
+      <c r="A56" s="55"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="55"/>
     </row>
     <row r="57" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="45"/>
+      <c r="A57" s="55"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="55"/>
     </row>
     <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="45"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="45"/>
+      <c r="A58" s="55"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="55"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="55"/>
     </row>
     <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="45"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
-      <c r="J59" s="45"/>
-      <c r="K59" s="45"/>
+      <c r="A59" s="55"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
+      <c r="K59" s="55"/>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="45"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="45"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="45"/>
+      <c r="A60" s="55"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="55"/>
+      <c r="I60" s="55"/>
+      <c r="J60" s="55"/>
+      <c r="K60" s="55"/>
     </row>
     <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15"/>

</xml_diff>